<commit_message>
Excel With TestCaseSource Attribute Added
</commit_message>
<xml_diff>
--- a/OpenEMRAutomation/TestData/open_emr_data.xlsx
+++ b/OpenEMRAutomation/TestData/open_emr_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\Unisys Aug 2023\AutomationSolution\OpenEMRAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30383F76-595F-4257-8563-6401CE49E217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCB6BB1-D434-410F-BD94-3B89A93BA7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C3B0792E-0540-4D80-9BF5-1E5DFCA1DB9F}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>physician</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E71C8C-EA9E-4776-85D1-64716E3FA490}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD8"/>
+      <selection activeCell="D4" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,10 +464,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -472,15 +478,29 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>